<commit_message>
actualizacion modelo 720 2
</commit_message>
<xml_diff>
--- a/templates/modelo_720.xlsx
+++ b/templates/modelo_720.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldela\Desktop\AccuMails\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34617\Desktop\AccuMails\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC36691-0983-4889-B605-699286877C47}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9117AB8-2364-4448-89B9-9358507C1A75}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="20124" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>EMAIL</t>
   </si>
@@ -31,9 +31,6 @@
     <t>SALDO_FINAL_MONEDA</t>
   </si>
   <si>
-    <t>PRIMER_INGRESO</t>
-  </si>
-  <si>
     <t>jose</t>
   </si>
   <si>
@@ -49,29 +46,46 @@
     <t>ACCOUNT_ID</t>
   </si>
   <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>ldelatorre@accuratequant.com</t>
-  </si>
-  <si>
-    <t>pepitro2</t>
-  </si>
-  <si>
     <t>ENVIO</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>ialonso@accuratequant.com</t>
+  </si>
+  <si>
+    <t>Accurate</t>
+  </si>
+  <si>
+    <t>Narciso</t>
+  </si>
+  <si>
+    <t>nvega@accuratequant.com</t>
+  </si>
+  <si>
+    <t>Angel Marcos</t>
+  </si>
+  <si>
+    <t>angelmarcosac@hotmail.com</t>
+  </si>
+  <si>
+    <t>2101928P</t>
+  </si>
+  <si>
+    <t>FECHA_PRIMER_INGRESO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,14 +223,6 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -562,67 +568,75 @@
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Millares" xfId="43" builtinId="3"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="43" xr:uid="{FB76E1E4-6863-4893-9A80-DD3FB274E91D}"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{FB76E1E4-6863-4893-9A80-DD3FB274E91D}"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -638,7 +652,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -934,94 +948,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.19921875" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="10.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>50000</v>
+      </c>
+      <c r="E2" s="6">
+        <v>42914</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>50000</v>
-      </c>
-      <c r="D2">
-        <v>50000</v>
-      </c>
-      <c r="E2">
-        <v>50000</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>684684</v>
-      </c>
-      <c r="D3">
-        <v>67498746</v>
-      </c>
-      <c r="E3">
-        <v>65465516</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="C3" s="3">
+        <v>134766.28795946107</v>
+      </c>
+      <c r="D3" s="3">
+        <v>142496.86528384281</v>
+      </c>
+      <c r="E3" s="6">
+        <v>42914</v>
+      </c>
+      <c r="F3" s="4">
+        <v>21085397</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="C4" s="3">
+        <v>25678.535509487221</v>
+      </c>
+      <c r="D4" s="3">
+        <v>28681.86829694323</v>
+      </c>
+      <c r="E4" s="6">
+        <v>42734</v>
+      </c>
+      <c r="F4" s="4">
+        <v>21084643</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3">
+        <v>31589.1139916393</v>
+      </c>
+      <c r="D5" s="3">
+        <v>33065.957772925765</v>
+      </c>
+      <c r="E5" s="6">
+        <v>42766</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{1C247EC1-7A50-407E-AF9D-1722C78B0A70}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>